<commit_message>
Changed: Fix I/O assignments.
</commit_message>
<xml_diff>
--- a/Electrical diagrams/IO assignment.xlsx
+++ b/Electrical diagrams/IO assignment.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\favier\Documents\GitHub\ControlPanel\Electrical diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nemehy\cloud\Nemehy\Informatique\Projets\Control Panel BO\Dépôt GIT\Electrical diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="IO Assignment" sheetId="4" r:id="rId1"/>
     <sheet name="Affectations IO" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -440,7 +440,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -905,7 +905,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -923,22 +932,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1327,7 +1327,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="54" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="51" t="s">
@@ -1384,7 +1384,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="50" t="s">
         <v>78</v>
       </c>
@@ -1401,7 +1401,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="49">
         <v>0</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="50">
         <v>1</v>
       </c>
@@ -1443,7 +1443,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="64"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="50" t="s">
         <v>28</v>
       </c>
@@ -1460,7 +1460,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="64"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="50" t="s">
         <v>29</v>
       </c>
@@ -1477,7 +1477,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="50">
         <v>4</v>
       </c>
@@ -1498,7 +1498,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="64"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="50">
         <v>5</v>
       </c>
@@ -1519,7 +1519,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="50">
         <v>6</v>
       </c>
@@ -1540,7 +1540,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="64"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="50">
         <v>7</v>
       </c>
@@ -1561,7 +1561,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="50">
         <v>8</v>
       </c>
@@ -1582,7 +1582,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="50">
         <v>9</v>
       </c>
@@ -1603,7 +1603,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="50">
         <v>10</v>
       </c>
@@ -1624,7 +1624,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="64"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="50">
         <v>16</v>
       </c>
@@ -1645,7 +1645,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="50">
         <v>14</v>
       </c>
@@ -1666,7 +1666,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="64"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="50">
         <v>15</v>
       </c>
@@ -1680,14 +1680,14 @@
         <v>107</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G17" s="35">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="50">
         <v>18</v>
       </c>
@@ -1708,7 +1708,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="64"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="50">
         <v>19</v>
       </c>
@@ -1722,14 +1722,14 @@
         <v>107</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G19" s="35">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="64"/>
+      <c r="A20" s="56"/>
       <c r="B20" s="50">
         <v>20</v>
       </c>
@@ -1750,7 +1750,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="52" t="s">
         <v>39</v>
       </c>
@@ -1771,13 +1771,13 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="58"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="26" t="s">
         <v>52</v>
       </c>
@@ -1792,11 +1792,11 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="59" t="s">
+      <c r="A23" s="59"/>
+      <c r="B23" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="59"/>
+      <c r="C23" s="62"/>
       <c r="D23" s="50" t="s">
         <v>52</v>
       </c>
@@ -1811,11 +1811,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
-      <c r="B24" s="59" t="s">
+      <c r="A24" s="59"/>
+      <c r="B24" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="59"/>
+      <c r="C24" s="62"/>
       <c r="D24" s="50" t="s">
         <v>52</v>
       </c>
@@ -1830,11 +1830,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
-      <c r="B25" s="59" t="s">
+      <c r="A25" s="59"/>
+      <c r="B25" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="59"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="50" t="s">
         <v>52</v>
       </c>
@@ -1849,11 +1849,11 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
-      <c r="B26" s="59" t="s">
+      <c r="A26" s="59"/>
+      <c r="B26" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="59"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="50" t="s">
         <v>52</v>
       </c>
@@ -1868,11 +1868,11 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
-      <c r="B27" s="59" t="s">
+      <c r="A27" s="59"/>
+      <c r="B27" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="59"/>
+      <c r="C27" s="62"/>
       <c r="D27" s="50" t="s">
         <v>52</v>
       </c>
@@ -1887,11 +1887,11 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
-      <c r="B28" s="59" t="s">
+      <c r="A28" s="59"/>
+      <c r="B28" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="59"/>
+      <c r="C28" s="62"/>
       <c r="D28" s="50" t="s">
         <v>52</v>
       </c>
@@ -1906,11 +1906,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
-      <c r="B29" s="59" t="s">
+      <c r="A29" s="59"/>
+      <c r="B29" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="59"/>
+      <c r="C29" s="62"/>
       <c r="D29" s="50" t="s">
         <v>52</v>
       </c>
@@ -1925,11 +1925,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="57"/>
-      <c r="B30" s="54" t="s">
+      <c r="A30" s="60"/>
+      <c r="B30" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="54"/>
+      <c r="C30" s="63"/>
       <c r="D30" s="49" t="s">
         <v>52</v>
       </c>
@@ -1938,13 +1938,13 @@
       <c r="G30" s="39"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="55" t="s">
+      <c r="A31" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="58"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="15" t="s">
         <v>52</v>
       </c>
@@ -1959,11 +1959,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
-      <c r="B32" s="59" t="s">
+      <c r="A32" s="59"/>
+      <c r="B32" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="59"/>
+      <c r="C32" s="62"/>
       <c r="D32" s="50" t="s">
         <v>52</v>
       </c>
@@ -1978,11 +1978,11 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="56"/>
-      <c r="B33" s="59" t="s">
+      <c r="A33" s="59"/>
+      <c r="B33" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="59"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="50" t="s">
         <v>52</v>
       </c>
@@ -1997,11 +1997,11 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
-      <c r="B34" s="59" t="s">
+      <c r="A34" s="59"/>
+      <c r="B34" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="59"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="50" t="s">
         <v>52</v>
       </c>
@@ -2016,11 +2016,11 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
-      <c r="B35" s="59" t="s">
+      <c r="A35" s="59"/>
+      <c r="B35" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="59"/>
+      <c r="C35" s="62"/>
       <c r="D35" s="50" t="s">
         <v>52</v>
       </c>
@@ -2035,11 +2035,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
-      <c r="B36" s="59" t="s">
+      <c r="A36" s="59"/>
+      <c r="B36" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="59"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="50" t="s">
         <v>52</v>
       </c>
@@ -2054,11 +2054,11 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="59" t="s">
+      <c r="A37" s="59"/>
+      <c r="B37" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="59"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="50" t="s">
         <v>52</v>
       </c>
@@ -2073,11 +2073,11 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
-      <c r="B38" s="59" t="s">
+      <c r="A38" s="59"/>
+      <c r="B38" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="59"/>
+      <c r="C38" s="62"/>
       <c r="D38" s="50" t="s">
         <v>52</v>
       </c>
@@ -2092,11 +2092,11 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="57"/>
-      <c r="B39" s="54" t="s">
+      <c r="A39" s="60"/>
+      <c r="B39" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="54"/>
+      <c r="C39" s="63"/>
       <c r="D39" s="52" t="s">
         <v>52</v>
       </c>
@@ -2105,13 +2105,13 @@
       <c r="G39" s="39"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="60" t="s">
+      <c r="A40" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="61"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="26" t="s">
         <v>52</v>
       </c>
@@ -2126,11 +2126,11 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
-      <c r="B41" s="59" t="s">
+      <c r="A41" s="59"/>
+      <c r="B41" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="59"/>
+      <c r="C41" s="62"/>
       <c r="D41" s="50" t="s">
         <v>52</v>
       </c>
@@ -2145,11 +2145,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="56"/>
-      <c r="B42" s="59" t="s">
+      <c r="A42" s="59"/>
+      <c r="B42" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="59"/>
+      <c r="C42" s="62"/>
       <c r="D42" s="50" t="s">
         <v>52</v>
       </c>
@@ -2164,11 +2164,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="56"/>
-      <c r="B43" s="59" t="s">
+      <c r="A43" s="59"/>
+      <c r="B43" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="59"/>
+      <c r="C43" s="62"/>
       <c r="D43" s="50" t="s">
         <v>52</v>
       </c>
@@ -2183,11 +2183,11 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="56"/>
-      <c r="B44" s="59" t="s">
+      <c r="A44" s="59"/>
+      <c r="B44" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="59"/>
+      <c r="C44" s="62"/>
       <c r="D44" s="50" t="s">
         <v>52</v>
       </c>
@@ -2202,11 +2202,11 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="56"/>
-      <c r="B45" s="59" t="s">
+      <c r="A45" s="59"/>
+      <c r="B45" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="59"/>
+      <c r="C45" s="62"/>
       <c r="D45" s="50" t="s">
         <v>52</v>
       </c>
@@ -2221,11 +2221,11 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="56"/>
-      <c r="B46" s="59" t="s">
+      <c r="A46" s="59"/>
+      <c r="B46" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="59"/>
+      <c r="C46" s="62"/>
       <c r="D46" s="50" t="s">
         <v>52</v>
       </c>
@@ -2240,11 +2240,11 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="56"/>
-      <c r="B47" s="59" t="s">
+      <c r="A47" s="59"/>
+      <c r="B47" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="59"/>
+      <c r="C47" s="62"/>
       <c r="D47" s="50" t="s">
         <v>52</v>
       </c>
@@ -2259,11 +2259,11 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="57"/>
-      <c r="B48" s="54" t="s">
+      <c r="A48" s="60"/>
+      <c r="B48" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="54"/>
+      <c r="C48" s="63"/>
       <c r="D48" s="49" t="s">
         <v>52</v>
       </c>
@@ -2272,13 +2272,13 @@
       <c r="G48" s="39"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="58" t="s">
+      <c r="B49" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="58"/>
+      <c r="C49" s="61"/>
       <c r="D49" s="15" t="s">
         <v>52</v>
       </c>
@@ -2293,11 +2293,11 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="56"/>
-      <c r="B50" s="59" t="s">
+      <c r="A50" s="59"/>
+      <c r="B50" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="59"/>
+      <c r="C50" s="62"/>
       <c r="D50" s="50" t="s">
         <v>52</v>
       </c>
@@ -2312,11 +2312,11 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="56"/>
-      <c r="B51" s="59" t="s">
+      <c r="A51" s="59"/>
+      <c r="B51" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="59"/>
+      <c r="C51" s="62"/>
       <c r="D51" s="50" t="s">
         <v>52</v>
       </c>
@@ -2331,11 +2331,11 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="56"/>
-      <c r="B52" s="59" t="s">
+      <c r="A52" s="59"/>
+      <c r="B52" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="59"/>
+      <c r="C52" s="62"/>
       <c r="D52" s="50" t="s">
         <v>52</v>
       </c>
@@ -2350,11 +2350,11 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="56"/>
-      <c r="B53" s="59" t="s">
+      <c r="A53" s="59"/>
+      <c r="B53" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="59"/>
+      <c r="C53" s="62"/>
       <c r="D53" s="50" t="s">
         <v>52</v>
       </c>
@@ -2369,11 +2369,11 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="56"/>
-      <c r="B54" s="59" t="s">
+      <c r="A54" s="59"/>
+      <c r="B54" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="59"/>
+      <c r="C54" s="62"/>
       <c r="D54" s="50" t="s">
         <v>52</v>
       </c>
@@ -2388,11 +2388,11 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="56"/>
-      <c r="B55" s="59" t="s">
+      <c r="A55" s="59"/>
+      <c r="B55" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="59"/>
+      <c r="C55" s="62"/>
       <c r="D55" s="50" t="s">
         <v>52</v>
       </c>
@@ -2407,11 +2407,11 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="56"/>
-      <c r="B56" s="59" t="s">
+      <c r="A56" s="59"/>
+      <c r="B56" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="59"/>
+      <c r="C56" s="62"/>
       <c r="D56" s="50" t="s">
         <v>52</v>
       </c>
@@ -2420,11 +2420,11 @@
       <c r="G56" s="38"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="57"/>
-      <c r="B57" s="54" t="s">
+      <c r="A57" s="60"/>
+      <c r="B57" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="54"/>
+      <c r="C57" s="63"/>
       <c r="D57" s="49" t="s">
         <v>52</v>
       </c>
@@ -2433,13 +2433,13 @@
       <c r="G57" s="39"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="55" t="s">
+      <c r="A58" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="58" t="s">
+      <c r="B58" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="58"/>
+      <c r="C58" s="61"/>
       <c r="D58" s="15" t="s">
         <v>52</v>
       </c>
@@ -2454,11 +2454,11 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="56"/>
-      <c r="B59" s="59" t="s">
+      <c r="A59" s="59"/>
+      <c r="B59" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="59"/>
+      <c r="C59" s="62"/>
       <c r="D59" s="50" t="s">
         <v>52</v>
       </c>
@@ -2473,11 +2473,11 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="56"/>
-      <c r="B60" s="59" t="s">
+      <c r="A60" s="59"/>
+      <c r="B60" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C60" s="59"/>
+      <c r="C60" s="62"/>
       <c r="D60" s="50" t="s">
         <v>52</v>
       </c>
@@ -2492,11 +2492,11 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="56"/>
-      <c r="B61" s="59" t="s">
+      <c r="A61" s="59"/>
+      <c r="B61" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C61" s="59"/>
+      <c r="C61" s="62"/>
       <c r="D61" s="50" t="s">
         <v>52</v>
       </c>
@@ -2511,11 +2511,11 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="56"/>
-      <c r="B62" s="59" t="s">
+      <c r="A62" s="59"/>
+      <c r="B62" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C62" s="59"/>
+      <c r="C62" s="62"/>
       <c r="D62" s="50" t="s">
         <v>52</v>
       </c>
@@ -2530,11 +2530,11 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="56"/>
-      <c r="B63" s="59" t="s">
+      <c r="A63" s="59"/>
+      <c r="B63" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C63" s="59"/>
+      <c r="C63" s="62"/>
       <c r="D63" s="50" t="s">
         <v>52</v>
       </c>
@@ -2549,11 +2549,11 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="56"/>
-      <c r="B64" s="59" t="s">
+      <c r="A64" s="59"/>
+      <c r="B64" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="59"/>
+      <c r="C64" s="62"/>
       <c r="D64" s="50" t="s">
         <v>52</v>
       </c>
@@ -2562,11 +2562,11 @@
       <c r="G64" s="38"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="56"/>
-      <c r="B65" s="59" t="s">
+      <c r="A65" s="59"/>
+      <c r="B65" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="59"/>
+      <c r="C65" s="62"/>
       <c r="D65" s="50" t="s">
         <v>52</v>
       </c>
@@ -2575,11 +2575,11 @@
       <c r="G65" s="38"/>
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="57"/>
-      <c r="B66" s="54" t="s">
+      <c r="A66" s="60"/>
+      <c r="B66" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C66" s="54"/>
+      <c r="C66" s="63"/>
       <c r="D66" s="52" t="s">
         <v>52</v>
       </c>
@@ -2590,6 +2590,46 @@
     <row r="67" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="A58:A66"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A49:A57"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A40:A48"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="A31:A39"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
     <mergeCell ref="A2:A21"/>
     <mergeCell ref="A22:A30"/>
     <mergeCell ref="B22:C22"/>
@@ -2601,46 +2641,6 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A31:A39"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="A40:A48"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="A49:A57"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="A58:A66"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2691,7 +2691,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="54" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -2710,7 +2710,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="63"/>
+      <c r="A3" s="55"/>
       <c r="B3" s="18" t="s">
         <v>78</v>
       </c>
@@ -2727,7 +2727,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="63"/>
+      <c r="A4" s="55"/>
       <c r="B4" s="11">
         <v>0</v>
       </c>
@@ -2748,7 +2748,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="64"/>
+      <c r="A5" s="56"/>
       <c r="B5" s="18">
         <v>1</v>
       </c>
@@ -2769,7 +2769,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="64"/>
+      <c r="A6" s="56"/>
       <c r="B6" s="18" t="s">
         <v>28</v>
       </c>
@@ -2786,7 +2786,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="64"/>
+      <c r="A7" s="56"/>
       <c r="B7" s="18" t="s">
         <v>29</v>
       </c>
@@ -2803,7 +2803,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
+      <c r="A8" s="56"/>
       <c r="B8" s="18">
         <v>4</v>
       </c>
@@ -2824,7 +2824,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="64"/>
+      <c r="A9" s="56"/>
       <c r="B9" s="18">
         <v>5</v>
       </c>
@@ -2845,7 +2845,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="64"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="18">
         <v>6</v>
       </c>
@@ -2866,7 +2866,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="64"/>
+      <c r="A11" s="56"/>
       <c r="B11" s="18">
         <v>7</v>
       </c>
@@ -2887,7 +2887,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
+      <c r="A12" s="56"/>
       <c r="B12" s="18">
         <v>8</v>
       </c>
@@ -2908,7 +2908,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
+      <c r="A13" s="56"/>
       <c r="B13" s="18">
         <v>9</v>
       </c>
@@ -2929,7 +2929,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
+      <c r="A14" s="56"/>
       <c r="B14" s="18">
         <v>10</v>
       </c>
@@ -2950,7 +2950,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="64"/>
+      <c r="A15" s="56"/>
       <c r="B15" s="18">
         <v>16</v>
       </c>
@@ -2971,7 +2971,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
+      <c r="A16" s="56"/>
       <c r="B16" s="18">
         <v>14</v>
       </c>
@@ -2992,7 +2992,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="64"/>
+      <c r="A17" s="56"/>
       <c r="B17" s="18">
         <v>15</v>
       </c>
@@ -3013,7 +3013,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="64"/>
+      <c r="A18" s="56"/>
       <c r="B18" s="18">
         <v>18</v>
       </c>
@@ -3034,7 +3034,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="64"/>
+      <c r="A19" s="56"/>
       <c r="B19" s="18">
         <v>19</v>
       </c>
@@ -3055,7 +3055,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="64"/>
+      <c r="A20" s="56"/>
       <c r="B20" s="18">
         <v>20</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="57"/>
       <c r="B21" s="19" t="s">
         <v>39</v>
       </c>
@@ -3097,13 +3097,13 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
+      <c r="A22" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="58"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="26" t="s">
         <v>52</v>
       </c>
@@ -3118,11 +3118,11 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="56"/>
-      <c r="B23" s="59" t="s">
+      <c r="A23" s="59"/>
+      <c r="B23" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="59"/>
+      <c r="C23" s="62"/>
       <c r="D23" s="7" t="s">
         <v>52</v>
       </c>
@@ -3137,11 +3137,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="56"/>
-      <c r="B24" s="59" t="s">
+      <c r="A24" s="59"/>
+      <c r="B24" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="59"/>
+      <c r="C24" s="62"/>
       <c r="D24" s="7" t="s">
         <v>52</v>
       </c>
@@ -3156,11 +3156,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
-      <c r="B25" s="59" t="s">
+      <c r="A25" s="59"/>
+      <c r="B25" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="59"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="7" t="s">
         <v>52</v>
       </c>
@@ -3175,11 +3175,11 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="56"/>
-      <c r="B26" s="59" t="s">
+      <c r="A26" s="59"/>
+      <c r="B26" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="59"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="7" t="s">
         <v>52</v>
       </c>
@@ -3194,11 +3194,11 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="56"/>
-      <c r="B27" s="59" t="s">
+      <c r="A27" s="59"/>
+      <c r="B27" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="59"/>
+      <c r="C27" s="62"/>
       <c r="D27" s="7" t="s">
         <v>52</v>
       </c>
@@ -3213,11 +3213,11 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="56"/>
-      <c r="B28" s="59" t="s">
+      <c r="A28" s="59"/>
+      <c r="B28" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="59"/>
+      <c r="C28" s="62"/>
       <c r="D28" s="7" t="s">
         <v>52</v>
       </c>
@@ -3232,11 +3232,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="56"/>
-      <c r="B29" s="59" t="s">
+      <c r="A29" s="59"/>
+      <c r="B29" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="59"/>
+      <c r="C29" s="62"/>
       <c r="D29" s="7" t="s">
         <v>52</v>
       </c>
@@ -3251,11 +3251,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="57"/>
-      <c r="B30" s="54" t="s">
+      <c r="A30" s="60"/>
+      <c r="B30" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="54"/>
+      <c r="C30" s="63"/>
       <c r="D30" s="11" t="s">
         <v>52</v>
       </c>
@@ -3264,13 +3264,13 @@
       <c r="G30" s="39"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="55" t="s">
+      <c r="A31" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="58"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="15" t="s">
         <v>52</v>
       </c>
@@ -3285,11 +3285,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
-      <c r="B32" s="59" t="s">
+      <c r="A32" s="59"/>
+      <c r="B32" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="59"/>
+      <c r="C32" s="62"/>
       <c r="D32" s="7" t="s">
         <v>52</v>
       </c>
@@ -3304,11 +3304,11 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="56"/>
-      <c r="B33" s="59" t="s">
+      <c r="A33" s="59"/>
+      <c r="B33" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="59"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="7" t="s">
         <v>52</v>
       </c>
@@ -3323,11 +3323,11 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="56"/>
-      <c r="B34" s="59" t="s">
+      <c r="A34" s="59"/>
+      <c r="B34" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="59"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="7" t="s">
         <v>52</v>
       </c>
@@ -3342,11 +3342,11 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="56"/>
-      <c r="B35" s="59" t="s">
+      <c r="A35" s="59"/>
+      <c r="B35" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="59"/>
+      <c r="C35" s="62"/>
       <c r="D35" s="7" t="s">
         <v>52</v>
       </c>
@@ -3361,11 +3361,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="56"/>
-      <c r="B36" s="59" t="s">
+      <c r="A36" s="59"/>
+      <c r="B36" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="59"/>
+      <c r="C36" s="62"/>
       <c r="D36" s="7" t="s">
         <v>52</v>
       </c>
@@ -3380,11 +3380,11 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="56"/>
-      <c r="B37" s="59" t="s">
+      <c r="A37" s="59"/>
+      <c r="B37" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="59"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="7" t="s">
         <v>52</v>
       </c>
@@ -3399,11 +3399,11 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
-      <c r="B38" s="59" t="s">
+      <c r="A38" s="59"/>
+      <c r="B38" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="59"/>
+      <c r="C38" s="62"/>
       <c r="D38" s="7" t="s">
         <v>52</v>
       </c>
@@ -3418,11 +3418,11 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="57"/>
-      <c r="B39" s="54" t="s">
+      <c r="A39" s="60"/>
+      <c r="B39" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="54"/>
+      <c r="C39" s="63"/>
       <c r="D39" s="12" t="s">
         <v>52</v>
       </c>
@@ -3431,13 +3431,13 @@
       <c r="G39" s="39"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="60" t="s">
+      <c r="A40" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="61"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="26" t="s">
         <v>52</v>
       </c>
@@ -3452,11 +3452,11 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
-      <c r="B41" s="59" t="s">
+      <c r="A41" s="59"/>
+      <c r="B41" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="59"/>
+      <c r="C41" s="62"/>
       <c r="D41" s="7" t="s">
         <v>52</v>
       </c>
@@ -3471,11 +3471,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="56"/>
-      <c r="B42" s="59" t="s">
+      <c r="A42" s="59"/>
+      <c r="B42" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="59"/>
+      <c r="C42" s="62"/>
       <c r="D42" s="7" t="s">
         <v>52</v>
       </c>
@@ -3490,11 +3490,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="56"/>
-      <c r="B43" s="59" t="s">
+      <c r="A43" s="59"/>
+      <c r="B43" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="59"/>
+      <c r="C43" s="62"/>
       <c r="D43" s="7" t="s">
         <v>52</v>
       </c>
@@ -3509,11 +3509,11 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="56"/>
-      <c r="B44" s="59" t="s">
+      <c r="A44" s="59"/>
+      <c r="B44" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="59"/>
+      <c r="C44" s="62"/>
       <c r="D44" s="7" t="s">
         <v>52</v>
       </c>
@@ -3528,11 +3528,11 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="56"/>
-      <c r="B45" s="59" t="s">
+      <c r="A45" s="59"/>
+      <c r="B45" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="59"/>
+      <c r="C45" s="62"/>
       <c r="D45" s="7" t="s">
         <v>52</v>
       </c>
@@ -3547,11 +3547,11 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="56"/>
-      <c r="B46" s="59" t="s">
+      <c r="A46" s="59"/>
+      <c r="B46" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="59"/>
+      <c r="C46" s="62"/>
       <c r="D46" s="7" t="s">
         <v>52</v>
       </c>
@@ -3566,11 +3566,11 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="56"/>
-      <c r="B47" s="59" t="s">
+      <c r="A47" s="59"/>
+      <c r="B47" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="59"/>
+      <c r="C47" s="62"/>
       <c r="D47" s="7" t="s">
         <v>52</v>
       </c>
@@ -3585,11 +3585,11 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="57"/>
-      <c r="B48" s="54" t="s">
+      <c r="A48" s="60"/>
+      <c r="B48" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="54"/>
+      <c r="C48" s="63"/>
       <c r="D48" s="11" t="s">
         <v>52</v>
       </c>
@@ -3598,13 +3598,13 @@
       <c r="G48" s="39"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="55" t="s">
+      <c r="A49" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="58" t="s">
+      <c r="B49" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="58"/>
+      <c r="C49" s="61"/>
       <c r="D49" s="15" t="s">
         <v>52</v>
       </c>
@@ -3619,11 +3619,11 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="56"/>
-      <c r="B50" s="59" t="s">
+      <c r="A50" s="59"/>
+      <c r="B50" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="59"/>
+      <c r="C50" s="62"/>
       <c r="D50" s="7" t="s">
         <v>52</v>
       </c>
@@ -3638,11 +3638,11 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="56"/>
-      <c r="B51" s="59" t="s">
+      <c r="A51" s="59"/>
+      <c r="B51" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="59"/>
+      <c r="C51" s="62"/>
       <c r="D51" s="7" t="s">
         <v>52</v>
       </c>
@@ -3657,11 +3657,11 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="56"/>
-      <c r="B52" s="59" t="s">
+      <c r="A52" s="59"/>
+      <c r="B52" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="59"/>
+      <c r="C52" s="62"/>
       <c r="D52" s="7" t="s">
         <v>52</v>
       </c>
@@ -3676,11 +3676,11 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="56"/>
-      <c r="B53" s="59" t="s">
+      <c r="A53" s="59"/>
+      <c r="B53" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="59"/>
+      <c r="C53" s="62"/>
       <c r="D53" s="7" t="s">
         <v>52</v>
       </c>
@@ -3695,11 +3695,11 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="56"/>
-      <c r="B54" s="59" t="s">
+      <c r="A54" s="59"/>
+      <c r="B54" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="59"/>
+      <c r="C54" s="62"/>
       <c r="D54" s="7" t="s">
         <v>52</v>
       </c>
@@ -3714,11 +3714,11 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="56"/>
-      <c r="B55" s="59" t="s">
+      <c r="A55" s="59"/>
+      <c r="B55" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="59"/>
+      <c r="C55" s="62"/>
       <c r="D55" s="7" t="s">
         <v>52</v>
       </c>
@@ -3733,11 +3733,11 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="56"/>
-      <c r="B56" s="59" t="s">
+      <c r="A56" s="59"/>
+      <c r="B56" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="59"/>
+      <c r="C56" s="62"/>
       <c r="D56" s="7" t="s">
         <v>52</v>
       </c>
@@ -3746,11 +3746,11 @@
       <c r="G56" s="38"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="57"/>
-      <c r="B57" s="54" t="s">
+      <c r="A57" s="60"/>
+      <c r="B57" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="54"/>
+      <c r="C57" s="63"/>
       <c r="D57" s="11" t="s">
         <v>52</v>
       </c>
@@ -3759,13 +3759,13 @@
       <c r="G57" s="39"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="55" t="s">
+      <c r="A58" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="58" t="s">
+      <c r="B58" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="58"/>
+      <c r="C58" s="61"/>
       <c r="D58" s="15" t="s">
         <v>52</v>
       </c>
@@ -3780,11 +3780,11 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="56"/>
-      <c r="B59" s="59" t="s">
+      <c r="A59" s="59"/>
+      <c r="B59" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="59"/>
+      <c r="C59" s="62"/>
       <c r="D59" s="7" t="s">
         <v>52</v>
       </c>
@@ -3799,11 +3799,11 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="56"/>
-      <c r="B60" s="59" t="s">
+      <c r="A60" s="59"/>
+      <c r="B60" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C60" s="59"/>
+      <c r="C60" s="62"/>
       <c r="D60" s="7" t="s">
         <v>52</v>
       </c>
@@ -3818,11 +3818,11 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="56"/>
-      <c r="B61" s="59" t="s">
+      <c r="A61" s="59"/>
+      <c r="B61" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C61" s="59"/>
+      <c r="C61" s="62"/>
       <c r="D61" s="7" t="s">
         <v>52</v>
       </c>
@@ -3837,11 +3837,11 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="56"/>
-      <c r="B62" s="59" t="s">
+      <c r="A62" s="59"/>
+      <c r="B62" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C62" s="59"/>
+      <c r="C62" s="62"/>
       <c r="D62" s="7" t="s">
         <v>52</v>
       </c>
@@ -3856,11 +3856,11 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="56"/>
-      <c r="B63" s="59" t="s">
+      <c r="A63" s="59"/>
+      <c r="B63" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="C63" s="59"/>
+      <c r="C63" s="62"/>
       <c r="D63" s="7" t="s">
         <v>52</v>
       </c>
@@ -3875,11 +3875,11 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="56"/>
-      <c r="B64" s="59" t="s">
+      <c r="A64" s="59"/>
+      <c r="B64" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="59"/>
+      <c r="C64" s="62"/>
       <c r="D64" s="7" t="s">
         <v>52</v>
       </c>
@@ -3888,11 +3888,11 @@
       <c r="G64" s="38"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="56"/>
-      <c r="B65" s="59" t="s">
+      <c r="A65" s="59"/>
+      <c r="B65" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="59"/>
+      <c r="C65" s="62"/>
       <c r="D65" s="7" t="s">
         <v>52</v>
       </c>
@@ -3901,11 +3901,11 @@
       <c r="G65" s="38"/>
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="57"/>
-      <c r="B66" s="54" t="s">
+      <c r="A66" s="60"/>
+      <c r="B66" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="C66" s="54"/>
+      <c r="C66" s="63"/>
       <c r="D66" s="21" t="s">
         <v>52</v>
       </c>
@@ -3916,25 +3916,22 @@
     <row r="67" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A49:A57"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="A2:A21"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A31:A39"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="B48:C48"/>
@@ -3951,22 +3948,25 @@
     <mergeCell ref="B63:C63"/>
     <mergeCell ref="B65:C65"/>
     <mergeCell ref="B66:C66"/>
-    <mergeCell ref="A2:A21"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="A31:A39"/>
+    <mergeCell ref="A49:A57"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added: Create a Tab for Joystick assignment simpler view.
</commit_message>
<xml_diff>
--- a/Electrical diagrams/IO assignment.xlsx
+++ b/Electrical diagrams/IO assignment.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nemehy\cloud\Nemehy\Informatique\Projets\Control Panel BO\Dépôt GIT\Electrical diagrams\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Commun\Informatique\Projets\Control Panel BO\Dépôt GIT\Electrical diagrams\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC59BD6-6A02-4206-8B23-07F949F3322B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IO Assignment" sheetId="4" r:id="rId1"/>
     <sheet name="Affectations IO" sheetId="3" r:id="rId2"/>
+    <sheet name="Mapping des contrôles" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="135">
   <si>
     <t>Power on/off</t>
   </si>
@@ -440,7 +442,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -502,7 +504,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -758,11 +760,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -905,6 +950,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -917,28 +986,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1322,10 +1391,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
@@ -1365,7 +1434,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="62" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="51" t="s">
@@ -1384,7 +1453,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
+      <c r="A3" s="63"/>
       <c r="B3" s="50" t="s">
         <v>78</v>
       </c>
@@ -1401,7 +1470,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
+      <c r="A4" s="63"/>
       <c r="B4" s="49">
         <v>0</v>
       </c>
@@ -1422,7 +1491,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="50">
         <v>1</v>
       </c>
@@ -1443,7 +1512,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="50" t="s">
         <v>28</v>
       </c>
@@ -1460,7 +1529,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="50" t="s">
         <v>29</v>
       </c>
@@ -1477,7 +1546,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="50">
         <v>4</v>
       </c>
@@ -1498,7 +1567,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="50">
         <v>5</v>
       </c>
@@ -1519,7 +1588,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="50">
         <v>6</v>
       </c>
@@ -1540,7 +1609,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="50">
         <v>7</v>
       </c>
@@ -1561,7 +1630,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="50">
         <v>8</v>
       </c>
@@ -1582,7 +1651,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="50">
         <v>9</v>
       </c>
@@ -1603,7 +1672,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="50">
         <v>10</v>
       </c>
@@ -1624,7 +1693,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="50">
         <v>16</v>
       </c>
@@ -1645,7 +1714,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="50">
         <v>14</v>
       </c>
@@ -1666,7 +1735,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="50">
         <v>15</v>
       </c>
@@ -1687,7 +1756,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="50">
         <v>18</v>
       </c>
@@ -1708,7 +1777,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="50">
         <v>19</v>
       </c>
@@ -1729,7 +1798,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="50">
         <v>20</v>
       </c>
@@ -1750,7 +1819,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="57"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="52" t="s">
         <v>39</v>
       </c>
@@ -1771,13 +1840,13 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="61"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="26" t="s">
         <v>52</v>
       </c>
@@ -1792,11 +1861,11 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-      <c r="B23" s="62" t="s">
+      <c r="A23" s="56"/>
+      <c r="B23" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="62"/>
+      <c r="C23" s="59"/>
       <c r="D23" s="50" t="s">
         <v>52</v>
       </c>
@@ -1811,11 +1880,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="62" t="s">
+      <c r="A24" s="56"/>
+      <c r="B24" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="62"/>
+      <c r="C24" s="59"/>
       <c r="D24" s="50" t="s">
         <v>52</v>
       </c>
@@ -1830,11 +1899,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="62" t="s">
+      <c r="A25" s="56"/>
+      <c r="B25" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="62"/>
+      <c r="C25" s="59"/>
       <c r="D25" s="50" t="s">
         <v>52</v>
       </c>
@@ -1849,11 +1918,11 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
-      <c r="B26" s="62" t="s">
+      <c r="A26" s="56"/>
+      <c r="B26" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="62"/>
+      <c r="C26" s="59"/>
       <c r="D26" s="50" t="s">
         <v>52</v>
       </c>
@@ -1868,11 +1937,11 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
-      <c r="B27" s="62" t="s">
+      <c r="A27" s="56"/>
+      <c r="B27" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="62"/>
+      <c r="C27" s="59"/>
       <c r="D27" s="50" t="s">
         <v>52</v>
       </c>
@@ -1887,11 +1956,11 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
-      <c r="B28" s="62" t="s">
+      <c r="A28" s="56"/>
+      <c r="B28" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="62"/>
+      <c r="C28" s="59"/>
       <c r="D28" s="50" t="s">
         <v>52</v>
       </c>
@@ -1906,11 +1975,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
-      <c r="B29" s="62" t="s">
+      <c r="A29" s="56"/>
+      <c r="B29" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="62"/>
+      <c r="C29" s="59"/>
       <c r="D29" s="50" t="s">
         <v>52</v>
       </c>
@@ -1925,11 +1994,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="60"/>
-      <c r="B30" s="63" t="s">
+      <c r="A30" s="57"/>
+      <c r="B30" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="63"/>
+      <c r="C30" s="54"/>
       <c r="D30" s="49" t="s">
         <v>52</v>
       </c>
@@ -1938,13 +2007,13 @@
       <c r="G30" s="39"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="61"/>
+      <c r="C31" s="58"/>
       <c r="D31" s="15" t="s">
         <v>52</v>
       </c>
@@ -1959,11 +2028,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
-      <c r="B32" s="62" t="s">
+      <c r="A32" s="56"/>
+      <c r="B32" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="62"/>
+      <c r="C32" s="59"/>
       <c r="D32" s="50" t="s">
         <v>52</v>
       </c>
@@ -1978,11 +2047,11 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
-      <c r="B33" s="62" t="s">
+      <c r="A33" s="56"/>
+      <c r="B33" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="62"/>
+      <c r="C33" s="59"/>
       <c r="D33" s="50" t="s">
         <v>52</v>
       </c>
@@ -1997,11 +2066,11 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
-      <c r="B34" s="62" t="s">
+      <c r="A34" s="56"/>
+      <c r="B34" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="62"/>
+      <c r="C34" s="59"/>
       <c r="D34" s="50" t="s">
         <v>52</v>
       </c>
@@ -2016,11 +2085,11 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
-      <c r="B35" s="62" t="s">
+      <c r="A35" s="56"/>
+      <c r="B35" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="62"/>
+      <c r="C35" s="59"/>
       <c r="D35" s="50" t="s">
         <v>52</v>
       </c>
@@ -2035,11 +2104,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
-      <c r="B36" s="62" t="s">
+      <c r="A36" s="56"/>
+      <c r="B36" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="62"/>
+      <c r="C36" s="59"/>
       <c r="D36" s="50" t="s">
         <v>52</v>
       </c>
@@ -2054,11 +2123,11 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
-      <c r="B37" s="62" t="s">
+      <c r="A37" s="56"/>
+      <c r="B37" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="62"/>
+      <c r="C37" s="59"/>
       <c r="D37" s="50" t="s">
         <v>52</v>
       </c>
@@ -2073,11 +2142,11 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
-      <c r="B38" s="62" t="s">
+      <c r="A38" s="56"/>
+      <c r="B38" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="62"/>
+      <c r="C38" s="59"/>
       <c r="D38" s="50" t="s">
         <v>52</v>
       </c>
@@ -2092,11 +2161,11 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="60"/>
-      <c r="B39" s="63" t="s">
+      <c r="A39" s="57"/>
+      <c r="B39" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="63"/>
+      <c r="C39" s="54"/>
       <c r="D39" s="52" t="s">
         <v>52</v>
       </c>
@@ -2105,13 +2174,13 @@
       <c r="G39" s="39"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="65" t="s">
+      <c r="B40" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="65"/>
+      <c r="C40" s="61"/>
       <c r="D40" s="26" t="s">
         <v>52</v>
       </c>
@@ -2126,11 +2195,11 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="59"/>
-      <c r="B41" s="62" t="s">
+      <c r="A41" s="56"/>
+      <c r="B41" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="62"/>
+      <c r="C41" s="59"/>
       <c r="D41" s="50" t="s">
         <v>52</v>
       </c>
@@ -2145,11 +2214,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="59"/>
-      <c r="B42" s="62" t="s">
+      <c r="A42" s="56"/>
+      <c r="B42" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="62"/>
+      <c r="C42" s="59"/>
       <c r="D42" s="50" t="s">
         <v>52</v>
       </c>
@@ -2164,11 +2233,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="59"/>
-      <c r="B43" s="62" t="s">
+      <c r="A43" s="56"/>
+      <c r="B43" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="62"/>
+      <c r="C43" s="59"/>
       <c r="D43" s="50" t="s">
         <v>52</v>
       </c>
@@ -2183,11 +2252,11 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
-      <c r="B44" s="62" t="s">
+      <c r="A44" s="56"/>
+      <c r="B44" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="62"/>
+      <c r="C44" s="59"/>
       <c r="D44" s="50" t="s">
         <v>52</v>
       </c>
@@ -2202,11 +2271,11 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
-      <c r="B45" s="62" t="s">
+      <c r="A45" s="56"/>
+      <c r="B45" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="62"/>
+      <c r="C45" s="59"/>
       <c r="D45" s="50" t="s">
         <v>52</v>
       </c>
@@ -2221,11 +2290,11 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="59"/>
-      <c r="B46" s="62" t="s">
+      <c r="A46" s="56"/>
+      <c r="B46" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="62"/>
+      <c r="C46" s="59"/>
       <c r="D46" s="50" t="s">
         <v>52</v>
       </c>
@@ -2240,11 +2309,11 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
-      <c r="B47" s="62" t="s">
+      <c r="A47" s="56"/>
+      <c r="B47" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="62"/>
+      <c r="C47" s="59"/>
       <c r="D47" s="50" t="s">
         <v>52</v>
       </c>
@@ -2259,11 +2328,11 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="60"/>
-      <c r="B48" s="63" t="s">
+      <c r="A48" s="57"/>
+      <c r="B48" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="63"/>
+      <c r="C48" s="54"/>
       <c r="D48" s="49" t="s">
         <v>52</v>
       </c>
@@ -2272,13 +2341,13 @@
       <c r="G48" s="39"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="58" t="s">
+      <c r="A49" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="61"/>
+      <c r="C49" s="58"/>
       <c r="D49" s="15" t="s">
         <v>52</v>
       </c>
@@ -2293,11 +2362,11 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="59"/>
-      <c r="B50" s="62" t="s">
+      <c r="A50" s="56"/>
+      <c r="B50" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="62"/>
+      <c r="C50" s="59"/>
       <c r="D50" s="50" t="s">
         <v>52</v>
       </c>
@@ -2312,11 +2381,11 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="59"/>
-      <c r="B51" s="62" t="s">
+      <c r="A51" s="56"/>
+      <c r="B51" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="62"/>
+      <c r="C51" s="59"/>
       <c r="D51" s="50" t="s">
         <v>52</v>
       </c>
@@ -2331,11 +2400,11 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="59"/>
-      <c r="B52" s="62" t="s">
+      <c r="A52" s="56"/>
+      <c r="B52" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="62"/>
+      <c r="C52" s="59"/>
       <c r="D52" s="50" t="s">
         <v>52</v>
       </c>
@@ -2350,11 +2419,11 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="59"/>
-      <c r="B53" s="62" t="s">
+      <c r="A53" s="56"/>
+      <c r="B53" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="62"/>
+      <c r="C53" s="59"/>
       <c r="D53" s="50" t="s">
         <v>52</v>
       </c>
@@ -2369,11 +2438,11 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="59"/>
-      <c r="B54" s="62" t="s">
+      <c r="A54" s="56"/>
+      <c r="B54" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="62"/>
+      <c r="C54" s="59"/>
       <c r="D54" s="50" t="s">
         <v>52</v>
       </c>
@@ -2388,11 +2457,11 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="59"/>
-      <c r="B55" s="62" t="s">
+      <c r="A55" s="56"/>
+      <c r="B55" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="62"/>
+      <c r="C55" s="59"/>
       <c r="D55" s="50" t="s">
         <v>52</v>
       </c>
@@ -2407,11 +2476,11 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="59"/>
-      <c r="B56" s="62" t="s">
+      <c r="A56" s="56"/>
+      <c r="B56" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="62"/>
+      <c r="C56" s="59"/>
       <c r="D56" s="50" t="s">
         <v>52</v>
       </c>
@@ -2420,11 +2489,11 @@
       <c r="G56" s="38"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="60"/>
-      <c r="B57" s="63" t="s">
+      <c r="A57" s="57"/>
+      <c r="B57" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="63"/>
+      <c r="C57" s="54"/>
       <c r="D57" s="49" t="s">
         <v>52</v>
       </c>
@@ -2433,13 +2502,13 @@
       <c r="G57" s="39"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="58" t="s">
+      <c r="A58" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="61" t="s">
+      <c r="B58" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="61"/>
+      <c r="C58" s="58"/>
       <c r="D58" s="15" t="s">
         <v>52</v>
       </c>
@@ -2454,11 +2523,11 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="59"/>
-      <c r="B59" s="62" t="s">
+      <c r="A59" s="56"/>
+      <c r="B59" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="62"/>
+      <c r="C59" s="59"/>
       <c r="D59" s="50" t="s">
         <v>52</v>
       </c>
@@ -2473,11 +2542,11 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="59"/>
-      <c r="B60" s="62" t="s">
+      <c r="A60" s="56"/>
+      <c r="B60" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C60" s="62"/>
+      <c r="C60" s="59"/>
       <c r="D60" s="50" t="s">
         <v>52</v>
       </c>
@@ -2492,11 +2561,11 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="59"/>
-      <c r="B61" s="62" t="s">
+      <c r="A61" s="56"/>
+      <c r="B61" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C61" s="62"/>
+      <c r="C61" s="59"/>
       <c r="D61" s="50" t="s">
         <v>52</v>
       </c>
@@ -2511,11 +2580,11 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="59"/>
-      <c r="B62" s="62" t="s">
+      <c r="A62" s="56"/>
+      <c r="B62" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C62" s="62"/>
+      <c r="C62" s="59"/>
       <c r="D62" s="50" t="s">
         <v>52</v>
       </c>
@@ -2530,11 +2599,11 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="59"/>
-      <c r="B63" s="62" t="s">
+      <c r="A63" s="56"/>
+      <c r="B63" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C63" s="62"/>
+      <c r="C63" s="59"/>
       <c r="D63" s="50" t="s">
         <v>52</v>
       </c>
@@ -2549,11 +2618,11 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="59"/>
-      <c r="B64" s="62" t="s">
+      <c r="A64" s="56"/>
+      <c r="B64" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="62"/>
+      <c r="C64" s="59"/>
       <c r="D64" s="50" t="s">
         <v>52</v>
       </c>
@@ -2562,11 +2631,11 @@
       <c r="G64" s="38"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="59"/>
-      <c r="B65" s="62" t="s">
+      <c r="A65" s="56"/>
+      <c r="B65" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="62"/>
+      <c r="C65" s="59"/>
       <c r="D65" s="50" t="s">
         <v>52</v>
       </c>
@@ -2575,11 +2644,11 @@
       <c r="G65" s="38"/>
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="60"/>
-      <c r="B66" s="63" t="s">
+      <c r="A66" s="57"/>
+      <c r="B66" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C66" s="63"/>
+      <c r="C66" s="54"/>
       <c r="D66" s="52" t="s">
         <v>52</v>
       </c>
@@ -2590,6 +2659,41 @@
     <row r="67" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="A2:A21"/>
+    <mergeCell ref="A22:A30"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A31:A39"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A40:A48"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
     <mergeCell ref="B66:C66"/>
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="A58:A66"/>
@@ -2606,41 +2710,6 @@
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A40:A48"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="A31:A39"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="A2:A21"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2648,12 +2717,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2691,7 +2760,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="62" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -2710,7 +2779,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
+      <c r="A3" s="63"/>
       <c r="B3" s="18" t="s">
         <v>78</v>
       </c>
@@ -2727,7 +2796,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
+      <c r="A4" s="63"/>
       <c r="B4" s="11">
         <v>0</v>
       </c>
@@ -2748,7 +2817,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="56"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="18">
         <v>1</v>
       </c>
@@ -2769,7 +2838,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="56"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="18" t="s">
         <v>28</v>
       </c>
@@ -2786,7 +2855,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="56"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="18" t="s">
         <v>29</v>
       </c>
@@ -2803,7 +2872,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="56"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="18">
         <v>4</v>
       </c>
@@ -2824,7 +2893,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="18">
         <v>5</v>
       </c>
@@ -2845,7 +2914,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="56"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="18">
         <v>6</v>
       </c>
@@ -2866,7 +2935,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="56"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="18">
         <v>7</v>
       </c>
@@ -2887,7 +2956,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="56"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="18">
         <v>8</v>
       </c>
@@ -2908,7 +2977,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="56"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="18">
         <v>9</v>
       </c>
@@ -2929,7 +2998,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="56"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="18">
         <v>10</v>
       </c>
@@ -2950,7 +3019,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="56"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="18">
         <v>16</v>
       </c>
@@ -2971,7 +3040,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="18">
         <v>14</v>
       </c>
@@ -2992,7 +3061,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="18">
         <v>15</v>
       </c>
@@ -3013,7 +3082,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="56"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="18">
         <v>18</v>
       </c>
@@ -3034,7 +3103,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="18">
         <v>19</v>
       </c>
@@ -3055,7 +3124,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="18">
         <v>20</v>
       </c>
@@ -3076,7 +3145,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="57"/>
+      <c r="A21" s="65"/>
       <c r="B21" s="19" t="s">
         <v>39</v>
       </c>
@@ -3097,13 +3166,13 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="61" t="s">
+      <c r="B22" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="61"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="26" t="s">
         <v>52</v>
       </c>
@@ -3118,11 +3187,11 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="59"/>
-      <c r="B23" s="62" t="s">
+      <c r="A23" s="56"/>
+      <c r="B23" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="62"/>
+      <c r="C23" s="59"/>
       <c r="D23" s="7" t="s">
         <v>52</v>
       </c>
@@ -3137,11 +3206,11 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="62" t="s">
+      <c r="A24" s="56"/>
+      <c r="B24" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="62"/>
+      <c r="C24" s="59"/>
       <c r="D24" s="7" t="s">
         <v>52</v>
       </c>
@@ -3156,11 +3225,11 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="59"/>
-      <c r="B25" s="62" t="s">
+      <c r="A25" s="56"/>
+      <c r="B25" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="62"/>
+      <c r="C25" s="59"/>
       <c r="D25" s="7" t="s">
         <v>52</v>
       </c>
@@ -3175,11 +3244,11 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="59"/>
-      <c r="B26" s="62" t="s">
+      <c r="A26" s="56"/>
+      <c r="B26" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="62"/>
+      <c r="C26" s="59"/>
       <c r="D26" s="7" t="s">
         <v>52</v>
       </c>
@@ -3194,11 +3263,11 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="59"/>
-      <c r="B27" s="62" t="s">
+      <c r="A27" s="56"/>
+      <c r="B27" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="62"/>
+      <c r="C27" s="59"/>
       <c r="D27" s="7" t="s">
         <v>52</v>
       </c>
@@ -3213,11 +3282,11 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="59"/>
-      <c r="B28" s="62" t="s">
+      <c r="A28" s="56"/>
+      <c r="B28" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="62"/>
+      <c r="C28" s="59"/>
       <c r="D28" s="7" t="s">
         <v>52</v>
       </c>
@@ -3232,11 +3301,11 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="59"/>
-      <c r="B29" s="62" t="s">
+      <c r="A29" s="56"/>
+      <c r="B29" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="62"/>
+      <c r="C29" s="59"/>
       <c r="D29" s="7" t="s">
         <v>52</v>
       </c>
@@ -3251,11 +3320,11 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="60"/>
-      <c r="B30" s="63" t="s">
+      <c r="A30" s="57"/>
+      <c r="B30" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="63"/>
+      <c r="C30" s="54"/>
       <c r="D30" s="11" t="s">
         <v>52</v>
       </c>
@@ -3264,13 +3333,13 @@
       <c r="G30" s="39"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="61"/>
+      <c r="C31" s="58"/>
       <c r="D31" s="15" t="s">
         <v>52</v>
       </c>
@@ -3285,11 +3354,11 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="59"/>
-      <c r="B32" s="62" t="s">
+      <c r="A32" s="56"/>
+      <c r="B32" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="62"/>
+      <c r="C32" s="59"/>
       <c r="D32" s="7" t="s">
         <v>52</v>
       </c>
@@ -3304,11 +3373,11 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="59"/>
-      <c r="B33" s="62" t="s">
+      <c r="A33" s="56"/>
+      <c r="B33" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="62"/>
+      <c r="C33" s="59"/>
       <c r="D33" s="7" t="s">
         <v>52</v>
       </c>
@@ -3323,11 +3392,11 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="59"/>
-      <c r="B34" s="62" t="s">
+      <c r="A34" s="56"/>
+      <c r="B34" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C34" s="62"/>
+      <c r="C34" s="59"/>
       <c r="D34" s="7" t="s">
         <v>52</v>
       </c>
@@ -3342,11 +3411,11 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="59"/>
-      <c r="B35" s="62" t="s">
+      <c r="A35" s="56"/>
+      <c r="B35" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="62"/>
+      <c r="C35" s="59"/>
       <c r="D35" s="7" t="s">
         <v>52</v>
       </c>
@@ -3361,11 +3430,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
-      <c r="B36" s="62" t="s">
+      <c r="A36" s="56"/>
+      <c r="B36" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="62"/>
+      <c r="C36" s="59"/>
       <c r="D36" s="7" t="s">
         <v>52</v>
       </c>
@@ -3380,11 +3449,11 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
-      <c r="B37" s="62" t="s">
+      <c r="A37" s="56"/>
+      <c r="B37" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="62"/>
+      <c r="C37" s="59"/>
       <c r="D37" s="7" t="s">
         <v>52</v>
       </c>
@@ -3399,11 +3468,11 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
-      <c r="B38" s="62" t="s">
+      <c r="A38" s="56"/>
+      <c r="B38" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C38" s="62"/>
+      <c r="C38" s="59"/>
       <c r="D38" s="7" t="s">
         <v>52</v>
       </c>
@@ -3418,11 +3487,11 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="60"/>
-      <c r="B39" s="63" t="s">
+      <c r="A39" s="57"/>
+      <c r="B39" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="63"/>
+      <c r="C39" s="54"/>
       <c r="D39" s="12" t="s">
         <v>52</v>
       </c>
@@ -3431,13 +3500,13 @@
       <c r="G39" s="39"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="65" t="s">
+      <c r="B40" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="65"/>
+      <c r="C40" s="61"/>
       <c r="D40" s="26" t="s">
         <v>52</v>
       </c>
@@ -3452,11 +3521,11 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="59"/>
-      <c r="B41" s="62" t="s">
+      <c r="A41" s="56"/>
+      <c r="B41" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="62"/>
+      <c r="C41" s="59"/>
       <c r="D41" s="7" t="s">
         <v>52</v>
       </c>
@@ -3471,11 +3540,11 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="59"/>
-      <c r="B42" s="62" t="s">
+      <c r="A42" s="56"/>
+      <c r="B42" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="62"/>
+      <c r="C42" s="59"/>
       <c r="D42" s="7" t="s">
         <v>52</v>
       </c>
@@ -3490,11 +3559,11 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="59"/>
-      <c r="B43" s="62" t="s">
+      <c r="A43" s="56"/>
+      <c r="B43" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="62"/>
+      <c r="C43" s="59"/>
       <c r="D43" s="7" t="s">
         <v>52</v>
       </c>
@@ -3509,11 +3578,11 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="59"/>
-      <c r="B44" s="62" t="s">
+      <c r="A44" s="56"/>
+      <c r="B44" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="62"/>
+      <c r="C44" s="59"/>
       <c r="D44" s="7" t="s">
         <v>52</v>
       </c>
@@ -3528,11 +3597,11 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="59"/>
-      <c r="B45" s="62" t="s">
+      <c r="A45" s="56"/>
+      <c r="B45" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="62"/>
+      <c r="C45" s="59"/>
       <c r="D45" s="7" t="s">
         <v>52</v>
       </c>
@@ -3547,11 +3616,11 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="59"/>
-      <c r="B46" s="62" t="s">
+      <c r="A46" s="56"/>
+      <c r="B46" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="62"/>
+      <c r="C46" s="59"/>
       <c r="D46" s="7" t="s">
         <v>52</v>
       </c>
@@ -3566,11 +3635,11 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="59"/>
-      <c r="B47" s="62" t="s">
+      <c r="A47" s="56"/>
+      <c r="B47" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="62"/>
+      <c r="C47" s="59"/>
       <c r="D47" s="7" t="s">
         <v>52</v>
       </c>
@@ -3585,11 +3654,11 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="60"/>
-      <c r="B48" s="63" t="s">
+      <c r="A48" s="57"/>
+      <c r="B48" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="63"/>
+      <c r="C48" s="54"/>
       <c r="D48" s="11" t="s">
         <v>52</v>
       </c>
@@ -3598,13 +3667,13 @@
       <c r="G48" s="39"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="58" t="s">
+      <c r="A49" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="61" t="s">
+      <c r="B49" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="61"/>
+      <c r="C49" s="58"/>
       <c r="D49" s="15" t="s">
         <v>52</v>
       </c>
@@ -3619,11 +3688,11 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="59"/>
-      <c r="B50" s="62" t="s">
+      <c r="A50" s="56"/>
+      <c r="B50" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="62"/>
+      <c r="C50" s="59"/>
       <c r="D50" s="7" t="s">
         <v>52</v>
       </c>
@@ -3638,11 +3707,11 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="59"/>
-      <c r="B51" s="62" t="s">
+      <c r="A51" s="56"/>
+      <c r="B51" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="62"/>
+      <c r="C51" s="59"/>
       <c r="D51" s="7" t="s">
         <v>52</v>
       </c>
@@ -3657,11 +3726,11 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="59"/>
-      <c r="B52" s="62" t="s">
+      <c r="A52" s="56"/>
+      <c r="B52" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="62"/>
+      <c r="C52" s="59"/>
       <c r="D52" s="7" t="s">
         <v>52</v>
       </c>
@@ -3676,11 +3745,11 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="59"/>
-      <c r="B53" s="62" t="s">
+      <c r="A53" s="56"/>
+      <c r="B53" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="62"/>
+      <c r="C53" s="59"/>
       <c r="D53" s="7" t="s">
         <v>52</v>
       </c>
@@ -3695,11 +3764,11 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="59"/>
-      <c r="B54" s="62" t="s">
+      <c r="A54" s="56"/>
+      <c r="B54" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C54" s="62"/>
+      <c r="C54" s="59"/>
       <c r="D54" s="7" t="s">
         <v>52</v>
       </c>
@@ -3714,11 +3783,11 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="59"/>
-      <c r="B55" s="62" t="s">
+      <c r="A55" s="56"/>
+      <c r="B55" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C55" s="62"/>
+      <c r="C55" s="59"/>
       <c r="D55" s="7" t="s">
         <v>52</v>
       </c>
@@ -3733,11 +3802,11 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="59"/>
-      <c r="B56" s="62" t="s">
+      <c r="A56" s="56"/>
+      <c r="B56" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="62"/>
+      <c r="C56" s="59"/>
       <c r="D56" s="7" t="s">
         <v>52</v>
       </c>
@@ -3746,11 +3815,11 @@
       <c r="G56" s="38"/>
     </row>
     <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="60"/>
-      <c r="B57" s="63" t="s">
+      <c r="A57" s="57"/>
+      <c r="B57" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="63"/>
+      <c r="C57" s="54"/>
       <c r="D57" s="11" t="s">
         <v>52</v>
       </c>
@@ -3759,13 +3828,13 @@
       <c r="G57" s="39"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="58" t="s">
+      <c r="A58" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="61" t="s">
+      <c r="B58" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="61"/>
+      <c r="C58" s="58"/>
       <c r="D58" s="15" t="s">
         <v>52</v>
       </c>
@@ -3780,11 +3849,11 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="59"/>
-      <c r="B59" s="62" t="s">
+      <c r="A59" s="56"/>
+      <c r="B59" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="62"/>
+      <c r="C59" s="59"/>
       <c r="D59" s="7" t="s">
         <v>52</v>
       </c>
@@ -3799,11 +3868,11 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="59"/>
-      <c r="B60" s="62" t="s">
+      <c r="A60" s="56"/>
+      <c r="B60" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="C60" s="62"/>
+      <c r="C60" s="59"/>
       <c r="D60" s="7" t="s">
         <v>52</v>
       </c>
@@ -3818,11 +3887,11 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="59"/>
-      <c r="B61" s="62" t="s">
+      <c r="A61" s="56"/>
+      <c r="B61" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="C61" s="62"/>
+      <c r="C61" s="59"/>
       <c r="D61" s="7" t="s">
         <v>52</v>
       </c>
@@ -3837,11 +3906,11 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="59"/>
-      <c r="B62" s="62" t="s">
+      <c r="A62" s="56"/>
+      <c r="B62" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="C62" s="62"/>
+      <c r="C62" s="59"/>
       <c r="D62" s="7" t="s">
         <v>52</v>
       </c>
@@ -3856,11 +3925,11 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="59"/>
-      <c r="B63" s="62" t="s">
+      <c r="A63" s="56"/>
+      <c r="B63" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="C63" s="62"/>
+      <c r="C63" s="59"/>
       <c r="D63" s="7" t="s">
         <v>52</v>
       </c>
@@ -3875,11 +3944,11 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="59"/>
-      <c r="B64" s="62" t="s">
+      <c r="A64" s="56"/>
+      <c r="B64" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="62"/>
+      <c r="C64" s="59"/>
       <c r="D64" s="7" t="s">
         <v>52</v>
       </c>
@@ -3888,11 +3957,11 @@
       <c r="G64" s="38"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="59"/>
-      <c r="B65" s="62" t="s">
+      <c r="A65" s="56"/>
+      <c r="B65" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="62"/>
+      <c r="C65" s="59"/>
       <c r="D65" s="7" t="s">
         <v>52</v>
       </c>
@@ -3901,11 +3970,11 @@
       <c r="G65" s="38"/>
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="60"/>
-      <c r="B66" s="63" t="s">
+      <c r="A66" s="57"/>
+      <c r="B66" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="C66" s="63"/>
+      <c r="C66" s="54"/>
       <c r="D66" s="21" t="s">
         <v>52</v>
       </c>
@@ -3916,6 +3985,41 @@
     <row r="67" spans="1:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="51">
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A49:A57"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="A40:A48"/>
+    <mergeCell ref="A58:A66"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
     <mergeCell ref="A2:A21"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
@@ -3932,44 +4036,421 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="A31:A39"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="A40:A48"/>
-    <mergeCell ref="A58:A66"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="A49:A57"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9127A75-60D7-426A-9AFA-DEC23E648E2D}">
+  <dimension ref="A1:B49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B49" sqref="A1:B49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="56" style="13" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="67">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="71" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="67">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="69" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="67">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="70">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="70">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="70">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="70">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="70">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="70">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="69" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="70">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="70">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" s="70">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="70">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="70">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="69" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="70">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="69" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="70">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="70">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="70">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="70">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="70">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="70">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="70">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="70">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="72" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="70">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="70">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="70">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="70">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="70">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="70">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" s="70">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="69" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="70">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="66" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="67" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="70" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="70" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="70" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" s="70" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="70" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" s="70" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="70" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="75" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>